<commit_message>
Actualizar diccionario de datos y MR
</commit_message>
<xml_diff>
--- a/Proyecto/Documentacion/Diccionario de datos.xlsx
+++ b/Proyecto/Documentacion/Diccionario de datos.xlsx
@@ -14,17 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="152">
   <si>
     <t>Administrativos</t>
   </si>
   <si>
+    <t>Campo</t>
+  </si>
+  <si>
+    <t>Programación</t>
+  </si>
+  <si>
     <t>Contratacion</t>
   </si>
   <si>
-    <t>Programación</t>
-  </si>
-  <si>
     <t>Contabilidad</t>
   </si>
   <si>
@@ -34,12 +37,24 @@
     <t>Electromecánica</t>
   </si>
   <si>
+    <t>Tipo de dato</t>
+  </si>
+  <si>
+    <t>Tamaño</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
     <t>Biología</t>
   </si>
   <si>
     <t>Tiempo completo</t>
   </si>
   <si>
+    <t>Usuario</t>
+  </si>
+  <si>
     <t>Comunicación</t>
   </si>
   <si>
@@ -52,6 +67,9 @@
     <t>Honorarios</t>
   </si>
   <si>
+    <t>IdUsuario</t>
+  </si>
+  <si>
     <t>Creatividad, procucción y diseño comercial</t>
   </si>
   <si>
@@ -64,6 +82,9 @@
     <t>Ingeniería</t>
   </si>
   <si>
+    <t>varchar</t>
+  </si>
+  <si>
     <t>Logística, transportación y distribución</t>
   </si>
   <si>
@@ -79,60 +100,39 @@
     <t>Salud y belleza</t>
   </si>
   <si>
+    <t>Identificador primario que garantiza unicidad</t>
+  </si>
+  <si>
     <t>Sector salud</t>
   </si>
   <si>
+    <t>Nombre</t>
+  </si>
+  <si>
     <t>Seguro y reaseguro</t>
   </si>
   <si>
+    <t>Nombre o nombres del usuario</t>
+  </si>
+  <si>
     <t>Tecnologías de la información / Sistemas</t>
   </si>
   <si>
     <t>Turismo, hospitalidad y gastronomía</t>
   </si>
   <si>
+    <t>APaterno</t>
+  </si>
+  <si>
     <t>Ventas</t>
   </si>
   <si>
+    <t>Apellido paterno del usuario</t>
+  </si>
+  <si>
     <t>Veterinaria / Zoología</t>
   </si>
   <si>
-    <t>Campo</t>
-  </si>
-  <si>
-    <t>Tipo de dato</t>
-  </si>
-  <si>
-    <t>Tamaño</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Usuario</t>
-  </si>
-  <si>
-    <t>IdUsuario</t>
-  </si>
-  <si>
-    <t>varchar</t>
-  </si>
-  <si>
-    <t>Identificador primario que garantiza unicidad</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Nombre o nombres del usuario</t>
-  </si>
-  <si>
-    <t>APaterno</t>
-  </si>
-  <si>
-    <t>Apellido paterno del usuario</t>
-  </si>
-  <si>
     <t>AMaterno</t>
   </si>
   <si>
@@ -154,22 +154,196 @@
     <t>Telefono</t>
   </si>
   <si>
+    <t>Numero de teléfono del usuario (incluye lada)</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Identificador primario que garantiza unicidad (RFC del director)</t>
+  </si>
+  <si>
+    <t>Nombre o nombres del director</t>
+  </si>
+  <si>
+    <t>Apellido paterno del director</t>
+  </si>
+  <si>
+    <t>Apellido materno del director</t>
+  </si>
+  <si>
+    <t>Correo electrónico del director</t>
+  </si>
+  <si>
     <t>numerico</t>
   </si>
   <si>
-    <t>Numero de teléfono del usuario (incluye lada)</t>
-  </si>
-  <si>
-    <t>Director</t>
-  </si>
-  <si>
-    <t>Identificador primario que garantiza unicidad (RFC del director)</t>
-  </si>
-  <si>
-    <t>Nombre o nombres del director</t>
-  </si>
-  <si>
-    <t>Apellido paterno del director</t>
+    <t>Numero de teléfono del director (incluye lada)</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Identificador primario que garantiza unicidad (RFC del administrador)</t>
+  </si>
+  <si>
+    <t>Nombre o nombres del administrador</t>
+  </si>
+  <si>
+    <t>Apellido paterno del administrador</t>
+  </si>
+  <si>
+    <t>Apellido materno del administrador</t>
+  </si>
+  <si>
+    <t>Sexo del administrador</t>
+  </si>
+  <si>
+    <t>Correo electrónico del administrador</t>
+  </si>
+  <si>
+    <t>Numero de teléfono del administrador (incluye lada)</t>
+  </si>
+  <si>
+    <t>Alumno</t>
+  </si>
+  <si>
+    <t>Identificador primario que garantiza unicidad (NoControl del alumno)</t>
+  </si>
+  <si>
+    <t>Nombre o nombres del alumno</t>
+  </si>
+  <si>
+    <t>Apellido paterno del alumno</t>
+  </si>
+  <si>
+    <t>Apelllido materno del alumno</t>
+  </si>
+  <si>
+    <t>Sexo del alumno</t>
+  </si>
+  <si>
+    <t>FechaNacimiento</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Fecha de nacimiento del alumno</t>
+  </si>
+  <si>
+    <t>Correo electrónico del alumno</t>
+  </si>
+  <si>
+    <t>Número de teléfono del alumno (incluyendo lada)</t>
+  </si>
+  <si>
+    <t>TelefonoCasa</t>
+  </si>
+  <si>
+    <t>Número de teléfono del alumno (teléfono de casa)</t>
+  </si>
+  <si>
+    <t>AreaInteres</t>
+  </si>
+  <si>
+    <t>El área de interés primordial del alumno para su desarrollo profesional</t>
+  </si>
+  <si>
+    <t>Encuesta</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>Almacena si el alumno contestó o no la encuesta, inicia en falso/0</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>IdGrupo</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>Identificador del grupo</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>El nombre del grupo (A,B,C,etc)</t>
+  </si>
+  <si>
+    <t>Especialidad</t>
+  </si>
+  <si>
+    <t>La especialidad del grupo (programación, contabilidad, electromecánica, arquitectura)</t>
+  </si>
+  <si>
+    <t>Turno</t>
+  </si>
+  <si>
+    <t>Turno del grupo (matutino o vespertino)</t>
+  </si>
+  <si>
+    <t>Semestre</t>
+  </si>
+  <si>
+    <t>Semestre en el que se encuentra el grupo (rango de  1 a 6)</t>
+  </si>
+  <si>
+    <t>Generacion</t>
+  </si>
+  <si>
+    <t>IdGeneracion</t>
+  </si>
+  <si>
+    <t>Identificador de la generación</t>
+  </si>
+  <si>
+    <t>FechaInicio</t>
+  </si>
+  <si>
+    <t>Fecha de inicio de la generación</t>
+  </si>
+  <si>
+    <t>FechaFin</t>
+  </si>
+  <si>
+    <t>Fecha en la que la genereación termina</t>
+  </si>
+  <si>
+    <t>IdEncuesta</t>
+  </si>
+  <si>
+    <t>Identificador de la encuesta</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Descripción que detalla a grandes razgos el enfoque de la encuesta</t>
+  </si>
+  <si>
+    <t>Activa</t>
+  </si>
+  <si>
+    <t>Designa si la encuesta se encuentra activa o inactiva</t>
+  </si>
+  <si>
+    <t>Archivo</t>
+  </si>
+  <si>
+    <t>Dirección del archivo que contiene la encuesta</t>
+  </si>
+  <si>
+    <t>Reporte</t>
   </si>
   <si>
     <t>Activo</t>
@@ -178,7 +352,10 @@
     <t>Es un alumno activo de la institución</t>
   </si>
   <si>
-    <t>Apellido materno del director</t>
+    <t>IdReporte</t>
+  </si>
+  <si>
+    <t>Identificador del reporte</t>
   </si>
   <si>
     <t>Trabajando</t>
@@ -187,213 +364,33 @@
     <t>El alumno se encuentra trabajando</t>
   </si>
   <si>
-    <t>Correo electrónico del director</t>
-  </si>
-  <si>
     <t>Universidad</t>
   </si>
   <si>
+    <t>Descripción a grandes razgos del reporte</t>
+  </si>
+  <si>
     <t>El alumno se encuentra estudiando de la universidad</t>
   </si>
   <si>
     <t>Prácticas</t>
   </si>
   <si>
-    <t>Numero de teléfono del director (incluye lada)</t>
-  </si>
-  <si>
     <t>El alumno se encuentra realizando sus prácticas profesionales</t>
   </si>
   <si>
+    <t>Dirección del archivo que contiene el reporte</t>
+  </si>
+  <si>
     <t>Egresado</t>
   </si>
   <si>
-    <t>Administrador</t>
+    <t>Fecha</t>
   </si>
   <si>
     <t>El alumno es egresado de la institución, pero no trabaja ni estudia</t>
   </si>
   <si>
-    <t>Identificador primario que garantiza unicidad (RFC del administrador)</t>
-  </si>
-  <si>
-    <t>Nombre o nombres del administrador</t>
-  </si>
-  <si>
-    <t>Apellido paterno del administrador</t>
-  </si>
-  <si>
-    <t>Apellido materno del administrador</t>
-  </si>
-  <si>
-    <t>Sexo del administrador</t>
-  </si>
-  <si>
-    <t>Correo electrónico del administrador</t>
-  </si>
-  <si>
-    <t>Numero de teléfono del administrador (incluye lada)</t>
-  </si>
-  <si>
-    <t>Alumno</t>
-  </si>
-  <si>
-    <t>Identificador primario que garantiza unicidad (NoControl del alumno)</t>
-  </si>
-  <si>
-    <t>Nombre o nombres del alumno</t>
-  </si>
-  <si>
-    <t>Apellido paterno del alumno</t>
-  </si>
-  <si>
-    <t>Apelllido materno del alumno</t>
-  </si>
-  <si>
-    <t>Sexo del alumno</t>
-  </si>
-  <si>
-    <t>FechaNacimiento</t>
-  </si>
-  <si>
-    <t>smalldatetime</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Fecha de nacimiento del alumno</t>
-  </si>
-  <si>
-    <t>Correo electrónico del alumno</t>
-  </si>
-  <si>
-    <t>numérico</t>
-  </si>
-  <si>
-    <t>Número de teléfono del alumno (incluyendo lada)</t>
-  </si>
-  <si>
-    <t>TelefonoCasa</t>
-  </si>
-  <si>
-    <t>Número de teléfono del alumno (teléfono de casa)</t>
-  </si>
-  <si>
-    <t>AreaInteres</t>
-  </si>
-  <si>
-    <t>El área de interés primordial del alumno para su desarrollo profesional</t>
-  </si>
-  <si>
-    <t>Encuesta</t>
-  </si>
-  <si>
-    <t>bit</t>
-  </si>
-  <si>
-    <t>Almacena si el alumno contestó o no la encuesta, inicia en falso/0</t>
-  </si>
-  <si>
-    <t>Grupo</t>
-  </si>
-  <si>
-    <t>IdGrupo</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>Identificador del grupo</t>
-  </si>
-  <si>
-    <t>char</t>
-  </si>
-  <si>
-    <t>El nombre del grupo (A,B,C,etc)</t>
-  </si>
-  <si>
-    <t>Especialidad</t>
-  </si>
-  <si>
-    <t>La especialidad del grupo (programación, contabilidad, electromecánica, arquitectura)</t>
-  </si>
-  <si>
-    <t>Turno</t>
-  </si>
-  <si>
-    <t>Turno del grupo (matutino o vespertino)</t>
-  </si>
-  <si>
-    <t>Semestre</t>
-  </si>
-  <si>
-    <t>Semestre en el que se encuentra el grupo (rango de  1 a 6)</t>
-  </si>
-  <si>
-    <t>Generacion</t>
-  </si>
-  <si>
-    <t>IdGeneracion</t>
-  </si>
-  <si>
-    <t>Identificador de la generación</t>
-  </si>
-  <si>
-    <t>FechaInicio</t>
-  </si>
-  <si>
-    <t>Fecha de inicio de la generación</t>
-  </si>
-  <si>
-    <t>FechaFin</t>
-  </si>
-  <si>
-    <t>Fecha en la que la genereación termina</t>
-  </si>
-  <si>
-    <t>IdEncuesta</t>
-  </si>
-  <si>
-    <t>Identificador de la encuesta</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>Descripción que detalla a grandes razgos el enfoque de la encuesta</t>
-  </si>
-  <si>
-    <t>Activa</t>
-  </si>
-  <si>
-    <t>Designa si la encuesta se encuentra activa o inactiva</t>
-  </si>
-  <si>
-    <t>Archivo</t>
-  </si>
-  <si>
-    <t>Dirección del archivo que contiene la encuesta</t>
-  </si>
-  <si>
-    <t>Reporte</t>
-  </si>
-  <si>
-    <t>IdReporte</t>
-  </si>
-  <si>
-    <t>Identificador del reporte</t>
-  </si>
-  <si>
-    <t>Descripción a grandes razgos del reporte</t>
-  </si>
-  <si>
-    <t>Dirección del archivo que contiene el reporte</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
     <t>Fecha en la que fué generado el reporte</t>
   </si>
   <si>
@@ -457,7 +454,7 @@
     <t>Identificador de la ocupación</t>
   </si>
   <si>
-    <t>Nombre de la ocupación</t>
+    <t>Nombre de la ocupación o del cargo</t>
   </si>
   <si>
     <t>Pequeña descripción de la ocupación</t>
@@ -466,7 +463,7 @@
     <t>AreaOcupacion</t>
   </si>
   <si>
-    <t>El área de ocupación del alumno (si es alumno Activo o Egresado, NA automático)</t>
+    <t>El área de ocupación del alumno(vease areaocupacion/interes)</t>
   </si>
   <si>
     <t>LugarOcupacion</t>
@@ -486,6 +483,9 @@
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="FF000000"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF2D2D2D"/>
@@ -500,9 +500,6 @@
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
-    </font>
-    <font>
       <strike/>
     </font>
   </fonts>
@@ -515,14 +512,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -546,22 +543,22 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
@@ -628,64 +625,64 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>30</v>
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
-        <v>31</v>
+      <c r="A2" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C3" s="9">
         <v>14.0</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C4" s="9">
         <v>50.0</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C5" s="9">
         <v>50.0</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
@@ -693,7 +690,7 @@
         <v>39</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C6" s="9">
         <v>50.0</v>
@@ -707,7 +704,7 @@
         <v>41</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C7" s="9">
         <v>10.0</v>
@@ -721,7 +718,7 @@
         <v>43</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C8" s="9">
         <v>100.0</v>
@@ -735,60 +732,60 @@
         <v>45</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C9" s="9">
         <v>13.0</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="11" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C11" s="12">
         <v>14.0</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C12" s="12">
         <v>30.0</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C13" s="12">
         <v>30.0</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
@@ -796,13 +793,13 @@
         <v>39</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C14" s="12">
         <v>30.0</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15">
@@ -810,13 +807,13 @@
         <v>43</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C15" s="12">
         <v>50.0</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16">
@@ -824,60 +821,60 @@
         <v>45</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C16" s="12">
         <v>13.0</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="11" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C18" s="12">
         <v>14.0</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C19" s="12">
         <v>30.0</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C20" s="12">
         <v>30.0</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21">
@@ -885,13 +882,13 @@
         <v>39</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C21" s="12">
         <v>30.0</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
@@ -899,13 +896,13 @@
         <v>41</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C22" s="12">
         <v>10.0</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23">
@@ -913,13 +910,13 @@
         <v>43</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C23" s="12">
         <v>50.0</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24">
@@ -927,60 +924,60 @@
         <v>45</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C24" s="12">
         <v>13.0</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
-        <v>73</v>
+      <c r="A25" s="6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C26" s="9">
         <v>14.0</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C27" s="9">
         <v>50.0</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C28" s="9">
         <v>50.0</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29">
@@ -988,13 +985,13 @@
         <v>39</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C29" s="9">
         <v>50.0</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30">
@@ -1002,27 +999,27 @@
         <v>41</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C30" s="9">
         <v>10.0</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32">
@@ -1030,13 +1027,13 @@
         <v>43</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C32" s="9">
-        <v>50.0</v>
+        <v>100.0</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33">
@@ -1044,515 +1041,515 @@
         <v>45</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="C33" s="9">
         <v>13.0</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C34" s="9">
         <v>13.0</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C35" s="9">
         <v>100.0</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="8" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C36" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="8" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="37">
-      <c r="A37" s="7" t="s">
-        <v>93</v>
+      <c r="A37" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C39" s="9">
         <v>1.0</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="8" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C40" s="9">
         <v>30.0</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="8" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C41" s="9">
         <v>1.0</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="8" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="7" t="s">
-        <v>105</v>
+      <c r="A43" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="8" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="8" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="8" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="7" t="s">
-        <v>90</v>
+      <c r="A47" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="8" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C48" s="9">
         <v>8.0</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C49" s="9">
         <v>100.0</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="8" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="8" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C51" s="9">
         <v>100.0</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="7" t="s">
-        <v>120</v>
+      <c r="A52" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="8" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C54" s="9">
         <v>200.0</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="8" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C55" s="9">
         <v>100.0</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B56" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" s="8" t="s">
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C59" s="9">
         <v>25.0</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C60" s="9">
         <v>100.0</v>
       </c>
       <c r="D60" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="7" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C63" s="9">
         <v>25.0</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C64" s="9">
         <v>100.0</v>
       </c>
       <c r="D64" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C67" s="9">
         <v>25.0</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C68" s="9">
         <v>100.0</v>
       </c>
       <c r="D68" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="7" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D70" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C71" s="9">
         <v>35.0</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="8" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C72" s="9">
         <v>200.0</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C73" s="9">
         <v>100.0</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C74" s="9">
         <v>100.0</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75">
@@ -7153,17 +7150,17 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -7188,116 +7185,116 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="D6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="D7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="D8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -7320,42 +7317,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>